<commit_message>
Added in Player Class and Map Class
Only added in the classes for the player and the map.
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l639\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l639\Desktop\SP3-Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>GunClass</t>
   </si>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,9 +428,10 @@
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +469,11 @@
       <c r="O1" t="s">
         <v>20</v>
       </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -483,7 +487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -494,7 +498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -505,7 +509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Merge with Weng Sang's map class fixes
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>GunClass</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>ObstacleClass</t>
+  </si>
+  <si>
+    <t>Vector2D</t>
   </si>
 </sst>
 </file>
@@ -410,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +434,7 @@
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +475,11 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -487,7 +493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -498,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -509,7 +515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>

</xml_diff>